<commit_message>
region header tooltip text done
I've got a working version of the tooltip that dynamically sizes for its text, I'm working on the svg world map to display the outlines
</commit_message>
<xml_diff>
--- a/BigOlTimeline_Data.xlsx
+++ b/BigOlTimeline_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\Personal\BigOlTimeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2840074E-4723-49CA-861C-B9C107BB2E91}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A4A607-99BF-420B-8B87-88D0A015A9C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17610" yWindow="4680" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChartBodyData" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="49">
   <si>
     <t>Ireland</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -385,8 +391,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F52EFD42-D6E2-4A08-8FE2-E75E0AB65E5F}" name="Table2" displayName="Table2" ref="A1:E93" totalsRowShown="0">
-  <autoFilter ref="A1:E93" xr:uid="{6C371244-143B-475C-BD39-3AA6BDBF30F8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F52EFD42-D6E2-4A08-8FE2-E75E0AB65E5F}" name="Table2" displayName="Table2" ref="A1:E94" totalsRowShown="0">
+  <autoFilter ref="A1:E94" xr:uid="{6C371244-143B-475C-BD39-3AA6BDBF30F8}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8FCFBCEA-948B-476D-9994-93EE35F50C77}" name="Index" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{EDBCC914-F39E-4F14-B20E-5B3EAAA4E167}" name="Region" dataDxfId="5"/>
@@ -689,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A5D2B2-EC0C-43BF-AEAB-FBB9B2CEBD8C}">
   <dimension ref="A1:T94"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G95" sqref="G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2538,6 +2544,21 @@
       <c r="I93" s="2"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="17">
+        <v>93</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D94" s="4">
+        <v>1</v>
+      </c>
+      <c r="E94" s="4">
+        <v>1</v>
+      </c>
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
     </row>
@@ -2554,8 +2575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13E63F6-A51F-4CC3-AEC2-DC0AACB4016F}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3040,7 +3061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239CDB62-EEB4-465F-85F6-D99E6B9E7D3B}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>

</xml_diff>